<commit_message>
may 5 2023 update
</commit_message>
<xml_diff>
--- a/db/uploads/gyrt import.xlsx
+++ b/db/uploads/gyrt import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaysonregalario/Desktop/project/cis_life_login-main/db/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920A8B4B-E1C6-E043-B3C3-82C06F10A10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D74774-8C4D-B545-ACE9-C19CFF75B3FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="3320" windowWidth="26040" windowHeight="14940" xr2:uid="{F8AE64F6-1B4E-984A-A10B-465BDBCF297A}"/>
+    <workbookView xWindow="2920" yWindow="2020" windowWidth="26040" windowHeight="14940" xr2:uid="{F8AE64F6-1B4E-984A-A10B-465BDBCF297A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6338,7 +6338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -6347,6 +6347,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6661,10 +6662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E00EFF-6865-D64D-92CF-647D20EDCF2D}">
-  <dimension ref="A1:H2400"/>
+  <dimension ref="A1:J2400"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:E2400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6678,7 +6679,7 @@
     <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6704,7 +6705,7 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6723,8 +6724,13 @@
       <c r="H2" s="5" t="s">
         <v>2067</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="8"/>
+      <c r="J2">
+        <f>COUNTIF(H:H,"*")</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -6743,8 +6749,12 @@
       <c r="H3" s="5" t="s">
         <v>2067</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <f>233.33*J2</f>
+        <v>559992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -6767,7 +6777,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -6787,7 +6797,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -6807,7 +6817,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -6824,7 +6834,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -6841,7 +6851,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -6858,7 +6868,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -6878,7 +6888,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -6898,7 +6908,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -6918,7 +6928,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -6941,7 +6951,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -6961,7 +6971,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -6981,7 +6991,7 @@
         <v>2067</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>

</xml_diff>